<commit_message>
Ubicación de audios finales LE_08_02_CO_REC250
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/SolicitudGrafica LE_08_02_REC310.xlsx
+++ b/fuentes/contenidos/grado08/guion02/SolicitudGrafica LE_08_02_REC310.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AULA PLANETA\PROCESO JUNIO 2015\GRADO OCTAVO\LE_08_02_CO\PROCESO OCTUBRE NUEVO\SOLICITUDES_GRAFICAS_02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luz Amparo\Documents\GitHub\Lenguaje\fuentes\contenidos\grado08\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -2180,14 +2180,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2652712</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>1488282</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2214562</xdr:colOff>
+      <xdr:colOff>2176462</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>45085</xdr:rowOff>
     </xdr:to>
@@ -2211,8 +2211,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16347281" y="12072938"/>
-          <a:ext cx="2190750" cy="568960"/>
+          <a:off x="16368712" y="13108782"/>
+          <a:ext cx="2190750" cy="576103"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2233,16 +2233,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>107156</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2647950</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1390650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>1309688</xdr:rowOff>
+      <xdr:colOff>1485900</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>242888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2264,8 +2264,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16430625" y="10679906"/>
-          <a:ext cx="1035844" cy="1214438"/>
+          <a:off x="16363950" y="11144250"/>
+          <a:ext cx="1504950" cy="2224088"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3057,9 +3057,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>